<commit_message>
Fix completion errors (#4)
</commit_message>
<xml_diff>
--- a/Tasks/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Tasks/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
   <si>
     <t xml:space="preserve">Echipa</t>
   </si>
@@ -115,34 +115,61 @@
     <t xml:space="preserve">01.03.2020</t>
   </si>
   <si>
-    <t xml:space="preserve">Decision logic is erroneous or inadequate.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coding Phase Defects Checklist/C01</t>
+    <t xml:space="preserve">C01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">src/main/java/tasks/services/TasksService.java / 15</t>
   </si>
   <si>
     <t xml:space="preserve">The TasksService would always use a local data source, meaning always querying the data that was in the storage file at the start of the application. Any changes to the file won’t be seen in the service (e.g. when a modified task would be the result of a filter, none of the changes would reflect in the result of the filter). Now the service always queries the data in the storage file.</t>
   </si>
   <si>
-    <t xml:space="preserve">Branching is erroneous.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coding Phase Defects Checklist/C02</t>
+    <t xml:space="preserve">C02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">src/main/java/tasks/model/Task.java / 100</t>
   </si>
   <si>
     <t xml:space="preserve">In the model folder, the Task class, the ‘nextTimeAfter’ method had a never reached ‘if’ branch.</t>
   </si>
   <si>
-    <t xml:space="preserve">There are errors in preparing or processing input data.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coding Phase Defects Checklist/C06</t>
+    <t xml:space="preserve">C03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">src/main/java/tasks/controller/Controller.java / 133</t>
   </si>
   <si>
     <t xml:space="preserve">When filtering tasks, if the user didn’t select both start and end date, the program wouldn’t display anything and throw errors in the console. Now if the user doesn’t select both dates, the application will display a messages box that tells the user that he/she has to provide both dates.</t>
   </si>
   <si>
-    <t xml:space="preserve">Effort to review document (hours): 0.5</t>
+    <t xml:space="preserve">C07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effort to review document (hours): 1.5</t>
   </si>
   <si>
     <t xml:space="preserve">do not print this form</t>
@@ -237,6 +264,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -254,13 +282,12 @@
       <family val="2"/>
     </font>
     <font>
-      <b val="true"/>
       <i val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="5">
@@ -351,7 +378,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -420,14 +447,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -452,7 +471,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -466,6 +485,30 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -687,8 +730,8 @@
         <v>2</v>
       </c>
       <c r="C11" s="15"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="16"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="6" t="n">
@@ -696,7 +739,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="15"/>
-      <c r="D12" s="17"/>
+      <c r="D12" s="15"/>
       <c r="E12" s="16"/>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -751,7 +794,7 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="19"/>
+      <c r="E18" s="17"/>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="6" t="n">
@@ -760,7 +803,7 @@
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="19"/>
+      <c r="E19" s="17"/>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="6" t="n">
@@ -769,7 +812,7 @@
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="19"/>
+      <c r="E20" s="17"/>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="6" t="n">
@@ -778,7 +821,7 @@
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="19"/>
+      <c r="E21" s="17"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="6" t="n">
@@ -787,7 +830,7 @@
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="19"/>
+      <c r="E22" s="17"/>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="6" t="n">
@@ -796,7 +839,7 @@
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="19"/>
+      <c r="E23" s="17"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="6" t="n">
@@ -805,7 +848,7 @@
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="19"/>
+      <c r="E24" s="17"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="6" t="n">
@@ -814,16 +857,16 @@
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="19"/>
+      <c r="E25" s="17"/>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E26" s="20"/>
+      <c r="E26" s="18"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="22"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="15"/>
     </row>
   </sheetData>
@@ -854,7 +897,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -864,7 +907,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="16.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="8.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="22.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="22.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="8.9"/>
   </cols>
   <sheetData>
@@ -904,13 +947,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="22"/>
       <c r="H4" s="6" t="s">
         <v>8</v>
       </c>
@@ -922,13 +965,13 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="23"/>
       <c r="H5" s="6" t="s">
         <v>12</v>
       </c>
@@ -1121,13 +1164,13 @@
       <c r="E26" s="16"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E27" s="20"/>
+      <c r="E27" s="18"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="22"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="15"/>
     </row>
   </sheetData>
@@ -1155,25 +1198,25 @@
     <tabColor rgb="FF8EB4E3"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="43.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="36.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="59.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="8.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="8.9"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="H1" s="4" t="s">
@@ -1182,7 +1225,7 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="s">
         <v>25</v>
       </c>
@@ -1209,13 +1252,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="25"/>
       <c r="H4" s="6" t="s">
         <v>8</v>
       </c>
@@ -1227,13 +1270,13 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="28"/>
+      <c r="E5" s="26"/>
       <c r="H5" s="6" t="s">
         <v>12</v>
       </c>
@@ -1244,7 +1287,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
         <v>14</v>
@@ -1254,7 +1297,7 @@
       </c>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="11" t="s">
         <v>15</v>
       </c>
@@ -1263,7 +1306,8 @@
       </c>
       <c r="E7" s="12"/>
     </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="13" t="s">
         <v>16</v>
       </c>
@@ -1278,83 +1322,175 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="123" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6" t="n">
+      <c r="B10" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="29" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="n">
+      <c r="B11" s="27" t="n">
         <f aca="false">B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="n">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="27" t="n">
         <f aca="false">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>38</v>
-      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="D13" s="0"/>
-      <c r="E13" s="0"/>
+      <c r="B13" s="27" t="n">
+        <f aca="false">B12+1</f>
+        <v>4</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="29"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0"/>
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
-      <c r="D14" s="0"/>
-      <c r="E14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="27" t="n">
+        <f aca="false">B13+1</f>
+        <v>5</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+    </row>
+    <row r="15" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0"/>
-      <c r="B15" s="0"/>
-      <c r="C15" s="21" t="s">
+      <c r="B15" s="27" t="n">
+        <f aca="false">B14+1</f>
+        <v>6</v>
+      </c>
+      <c r="C15" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="0"/>
-      <c r="E15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="D15" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="27" t="n">
+        <f aca="false">B15+1</f>
+        <v>7</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="27" t="n">
+        <f aca="false">B16+1</f>
+        <v>8</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="27" t="n">
+        <f aca="false">B17+1</f>
+        <v>9</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="27" t="n">
+        <f aca="false">B18+1</f>
+        <v>10</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="27" t="n">
+        <f aca="false">B19+1</f>
+        <v>11</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="27" t="n">
+        <f aca="false">B20+1</f>
+        <v>12</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0"/>
+      <c r="C22" s="0"/>
+      <c r="D22" s="0"/>
+      <c r="E22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0"/>
+      <c r="C23" s="0"/>
+      <c r="D23" s="0"/>
+      <c r="E23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0"/>
+      <c r="C24" s="0"/>
+      <c r="D24" s="0"/>
+      <c r="E24" s="0"/>
+    </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1408,7 +1544,7 @@
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>0</v>
@@ -1418,7 +1554,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1439,11 +1575,11 @@
       <c r="J3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="C4" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
       <c r="H4" s="6" t="s">
         <v>8</v>
       </c>
@@ -1475,16 +1611,16 @@
         <v>16</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1697,15 +1833,15 @@
       <c r="F30" s="16"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E31" s="20"/>
+      <c r="E31" s="18"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="30"/>
+      <c r="C32" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>